<commit_message>
remove MHCII codon usage graphing
not needed, all info is in codon_usage>coancestry_regression.R
</commit_message>
<xml_diff>
--- a/data/data and script readme info.xlsx
+++ b/data/data and script readme info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KatieMartin/Documents/UCF/Research/MHC_species_evo/Martin-et-al.-submitted/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{828A2E70-4600-ED45-8EF5-E17A860DA946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA34E8C-0D84-9A47-9AC8-640DAC65F3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13640" activeTab="1" xr2:uid="{419048BB-6B79-FA40-9B6F-5B1E63E224A5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="107">
   <si>
     <t>analysis</t>
   </si>
@@ -110,9 +110,6 @@
     <t>MHCI_supertype_input.csv</t>
   </si>
   <si>
-    <t>purpose</t>
-  </si>
-  <si>
     <t>selection analyses</t>
   </si>
   <si>
@@ -333,6 +330,33 @@
   </si>
   <si>
     <t>MHCI_allele_counts_for_rarefaction.csv, chr14_MHCII_allele_counts_for_rarefaction.csv, chr1_MHCII_allele_counts_for_rarefaction.csv</t>
+  </si>
+  <si>
+    <t>combined_MHCI_MHCII_allelic_div_stats_v4.csv</t>
+  </si>
+  <si>
+    <t>nucleotide diversity, number of alleles per species and per MHC region</t>
+  </si>
+  <si>
+    <t>combined_MHC_alleles_per_indiv_Cc_Cm_Dc_Lk.csv, combined_MHCI_MHCII_allelic_div_stats_v4.csv</t>
+  </si>
+  <si>
+    <t>removal of forward and reverse locus-specific primers from fastq files</t>
+  </si>
+  <si>
+    <t>fastq files raw (SRA)</t>
+  </si>
+  <si>
+    <t>nucleotide diversity calculations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allele_counts_by_species_supertypes_MHCI.csv, MHCI_infile.nex.con.tre, MHCI_IQTree.treefile, </t>
+  </si>
+  <si>
+    <t>visualization of gene tree</t>
+  </si>
+  <si>
+    <t>chr1_alm_for_nucdiv.fasta, chr14_alm_for_nucdiv.fasta</t>
   </si>
 </sst>
 </file>
@@ -382,11 +406,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DD37D5-7F48-1040-982C-A2C23FAB41E3}">
-  <dimension ref="B2:G45"/>
+  <dimension ref="B2:G46"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:B45"/>
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -720,7 +745,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -734,10 +759,10 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
@@ -746,63 +771,63 @@
         <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
         <v>5</v>
@@ -810,10 +835,10 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -827,10 +852,10 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -844,10 +869,10 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -861,10 +886,10 @@
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
@@ -878,10 +903,10 @@
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -898,7 +923,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" t="s">
         <v>9</v>
@@ -912,10 +937,10 @@
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
         <v>9</v>
@@ -927,52 +952,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="D16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
         <v>5</v>
@@ -980,16 +1005,16 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
         <v>5</v>
@@ -997,16 +1022,16 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
         <v>5</v>
@@ -1014,16 +1039,16 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D20" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
         <v>5</v>
@@ -1031,16 +1056,16 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>
@@ -1048,61 +1073,61 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>25</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>23</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="D22" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
+      <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D25" t="s">
         <v>52</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" t="s">
         <v>53</v>
-      </c>
-      <c r="E24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D27" t="s">
         <v>9</v>
@@ -1111,15 +1136,15 @@
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
         <v>9</v>
@@ -1128,15 +1153,15 @@
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D29" t="s">
         <v>9</v>
@@ -1145,15 +1170,15 @@
         <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
         <v>9</v>
@@ -1162,15 +1187,15 @@
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D31" t="s">
         <v>9</v>
@@ -1179,15 +1204,15 @@
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D32" t="s">
         <v>9</v>
@@ -1196,194 +1221,211 @@
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C33" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
         <v>52</v>
       </c>
-      <c r="D33" t="s">
-        <v>53</v>
-      </c>
-      <c r="E33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" t="s">
-        <v>73</v>
-      </c>
-      <c r="E35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" t="s">
-        <v>71</v>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="D36" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="E36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>74</v>
+      </c>
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" t="s">
         <v>70</v>
-      </c>
-      <c r="C37" t="s">
-        <v>83</v>
-      </c>
-      <c r="D37" t="s">
-        <v>34</v>
-      </c>
-      <c r="E37" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>84</v>
+        <v>67</v>
+      </c>
+      <c r="C40" t="s">
+        <v>76</v>
       </c>
       <c r="D40" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>84</v>
       </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C43" t="s">
-        <v>72</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" t="s">
-        <v>71</v>
+      <c r="C42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
+      </c>
+      <c r="E42" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="C44" t="s">
-        <v>47</v>
+        <v>71</v>
       </c>
       <c r="D44" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
         <v>32</v>
       </c>
-      <c r="E45" t="s">
-        <v>33</v>
-      </c>
       <c r="F45" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C46" t="s">
+        <v>46</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1396,36 +1438,43 @@
   <dimension ref="B2:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G8:K13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
@@ -1435,57 +1484,93 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>86</v>
+      </c>
+      <c r="C7" t="s">
+        <v>101</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="C8" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>6</v>
       </c>
+      <c r="C10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed lines pertaining to data viz
moved to new script
</commit_message>
<xml_diff>
--- a/data/data and script readme info.xlsx
+++ b/data/data and script readme info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/KatieMartin/Documents/UCF/Research/MHC_species_evo/Martin-et-al.-submitted/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEA34E8C-0D84-9A47-9AC8-640DAC65F3B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918712F-CE67-B142-A7A4-AC0A7584FA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="1000" windowWidth="25040" windowHeight="13640" activeTab="1" xr2:uid="{419048BB-6B79-FA40-9B6F-5B1E63E224A5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="115">
   <si>
     <t>analysis</t>
   </si>
@@ -302,15 +302,9 @@
     <t>dada2_primer_removal_MHCII_chr14.R</t>
   </si>
   <si>
-    <t>MHCII_codon_usage_graphing.R</t>
-  </si>
-  <si>
     <t>MHCII_combined_phylogeny.R</t>
   </si>
   <si>
-    <t>MHCII_supertyping_AMM.R</t>
-  </si>
-  <si>
     <t>supertyping_MHCII_combined.R</t>
   </si>
   <si>
@@ -357,6 +351,36 @@
   </si>
   <si>
     <t>chr1_alm_for_nucdiv.fasta, chr14_alm_for_nucdiv.fasta</t>
+  </si>
+  <si>
+    <t>codon usage analyes</t>
+  </si>
+  <si>
+    <t>lots lol</t>
+  </si>
+  <si>
+    <t>allele_counts_by_species_supertypes_MHCII.csv</t>
+  </si>
+  <si>
+    <t>MHCII_chr14_chr1_infile.nex.con.tre</t>
+  </si>
+  <si>
+    <t>iqtree_MHCIIcombined_15Sept24.contree</t>
+  </si>
+  <si>
+    <t>allele_counts_by_species_supertypes_MHCII.csv, MHCII_chr14_chr1_infile.nex.con.tre, iqtree_MHCIIcombined_15Sept24.contree</t>
+  </si>
+  <si>
+    <t>MHCII_combined_supertyping_input.csv</t>
+  </si>
+  <si>
+    <t>matrix of MHCII alleles with 5 'z' values for each amino acid</t>
+  </si>
+  <si>
+    <t>supertyping_MHCII.R</t>
+  </si>
+  <si>
+    <t>raw files (input to PEAR, once done with PEAR that's the input to DADA2) and input to amplisas (output from DADA2)</t>
   </si>
 </sst>
 </file>
@@ -406,12 +430,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -726,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87DD37D5-7F48-1040-982C-A2C23FAB41E3}">
-  <dimension ref="B2:G46"/>
+  <dimension ref="B1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,14 +763,20 @@
     <col min="3" max="3" width="58.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>2</v>
@@ -792,12 +823,12 @@
       </c>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>99</v>
+    <row r="5" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>40</v>
@@ -809,13 +840,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
+    <row r="6" spans="2:7" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>4</v>
@@ -969,20 +994,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="2:7" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1310,13 +1335,13 @@
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+      <c r="B39" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E39" t="s">
@@ -1327,13 +1352,13 @@
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="B40" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="5" t="s">
         <v>73</v>
       </c>
       <c r="E40" t="s">
@@ -1344,13 +1369,13 @@
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
+      <c r="B41" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C41" s="3" t="s">
+      <c r="C41" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E41" t="s">
@@ -1361,13 +1386,13 @@
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+      <c r="B42" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="5" t="s">
         <v>80</v>
       </c>
       <c r="E42" t="s">
@@ -1377,18 +1402,35 @@
         <v>70</v>
       </c>
     </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>65</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" t="s">
+        <v>70</v>
+      </c>
+    </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>65</v>
+        <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E44" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F44" t="s">
         <v>70</v>
@@ -1396,7 +1438,7 @@
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
         <v>46</v>
@@ -1413,18 +1455,69 @@
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C46" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D46" t="s">
-        <v>31</v>
+        <v>88</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F46" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
+        <v>88</v>
+      </c>
+      <c r="E47" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D48" t="s">
+        <v>88</v>
+      </c>
+      <c r="E48" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>111</v>
+      </c>
+      <c r="C49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D49" t="s">
+        <v>113</v>
+      </c>
+      <c r="E49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1435,10 +1528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D34A54F-D429-084B-879A-1094D57FECD1}">
-  <dimension ref="B2:D16"/>
+  <dimension ref="B2:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1449,10 +1542,10 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -1460,10 +1553,10 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
@@ -1474,23 +1567,29 @@
         <v>30</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
@@ -1498,10 +1597,10 @@
         <v>86</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
@@ -1509,10 +1608,10 @@
         <v>87</v>
       </c>
       <c r="C8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -1520,7 +1619,7 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9" t="s">
         <v>17</v>
@@ -1531,46 +1630,45 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>88</v>
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>89</v>
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>